<commit_message>
public school teacher age data
</commit_message>
<xml_diff>
--- a/final_project/sass_data/sass1112_18042404_t2n.xlsx
+++ b/final_project/sass_data/sass1112_18042404_t2n.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C389B5-A207-904A-A7DA-A74FB6C75BCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DED99E-A51D-294C-A18D-FEF5559F236F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="22">
   <si>
     <t>Level and selected subject area</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>!</t>
+  </si>
+  <si>
+    <t>‡</t>
   </si>
   <si>
     <t>Percentage of private school students in middle grade and high school departmentalized public school classes taught by a teacher certified in the subject area and percentage distribution of those students, by the teacher's certification and major status in selected subject areas: 2011-12</t>
@@ -586,7 +589,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -788,15 +791,21 @@
       <c r="A9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="E9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="G9" s="7" t="s">
         <v>15</v>
       </c>
@@ -804,7 +813,9 @@
         <v>60.7</v>
       </c>
       <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="J9" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="K9" s="5" t="s">
         <v>15</v>
       </c>
@@ -999,7 +1010,7 @@
     </row>
     <row r="16" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -1014,7 +1025,7 @@
     </row>
     <row r="17" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
@@ -1029,7 +1040,7 @@
     </row>
     <row r="18" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>

</xml_diff>